<commit_message>
add second person handling
</commit_message>
<xml_diff>
--- a/config_file/tixplus_ac.xlsx
+++ b/config_file/tixplus_ac.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/USER/Desktop/new_Fyp/lawson_auto/config_file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A98521-D186-AF4D-AAC9-CBA00B788C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667210DE-88CB-7046-A3CB-85C08C1D36EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="22340" windowWidth="28380" windowHeight="18380" xr2:uid="{BF0064B6-BD3E-834E-B1EC-9949E35C9C53}"/>
+    <workbookView xWindow="4460" yWindow="520" windowWidth="28380" windowHeight="18380" xr2:uid="{BF0064B6-BD3E-834E-B1EC-9949E35C9C53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>EMAIL</t>
   </si>
@@ -68,31 +65,34 @@
     <t>DOB</t>
   </si>
   <si>
-    <t>yyyy-mm-dd</t>
-  </si>
-  <si>
-    <t>xxx@sadasda.com</t>
-  </si>
-  <si>
-    <t>yourPw</t>
-  </si>
-  <si>
-    <t>陳</t>
-  </si>
-  <si>
-    <t>大文</t>
-  </si>
-  <si>
-    <t>チン</t>
-  </si>
-  <si>
-    <t>08011111111</t>
-  </si>
-  <si>
-    <t>E000000000000</t>
-  </si>
-  <si>
-    <t>ダイマン</t>
+    <t>MONTH</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>a123456</t>
+  </si>
+  <si>
+    <t>ヨシカワ</t>
+  </si>
+  <si>
+    <t>ショウ</t>
+  </si>
+  <si>
+    <t>1995-09-23</t>
+  </si>
+  <si>
+    <t>XXXX@dropmail.me</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>EXXXXXXXXXX</t>
   </si>
 </sst>
 </file>
@@ -483,21 +483,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5124B7D8-113B-0F41-9965-645E1A7CBEA5}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,108 +517,120 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
       <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
       <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2">
+        <v>9011111111</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>1995</v>
+      </c>
+      <c r="K2">
+        <v>9</v>
+      </c>
+      <c r="L2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="H3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="H4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="H5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="H6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="H7" s="2"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G7" s="2"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="H8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G10" s="2"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="H11" s="2"/>
-      <c r="J11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="I11" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{7C1B4D1B-9722-D947-8DFF-D05F5B89B4C3}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{88B4A8B8-A887-6B47-8B8E-0BD2B019A2CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>